<commit_message>
Added orderLine on cafeExercise
</commit_message>
<xml_diff>
--- a/cafeExercise.xlsx
+++ b/cafeExercise.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>CafePatreons</t>
   </si>
@@ -38,15 +38,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Order1</t>
-  </si>
-  <si>
-    <t>Order2</t>
-  </si>
-  <si>
-    <t>Order3</t>
-  </si>
-  <si>
     <t>Drinks</t>
   </si>
   <si>
@@ -107,19 +98,16 @@
     <t>Fanta</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>OrderPatreons</t>
   </si>
 </sst>
 </file>
@@ -180,29 +168,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F7" totalsRowShown="0">
-  <autoFilter ref="A2:F7"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:C7" totalsRowShown="0">
+  <autoFilter ref="A2:C7"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="PatreonID" dataDxfId="0"/>
     <tableColumn id="2" name="FirstName"/>
     <tableColumn id="3" name="LastName"/>
-    <tableColumn id="4" name="Order1"/>
-    <tableColumn id="5" name="Order2"/>
-    <tableColumn id="6" name="Order3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A12:C19" totalsRowShown="0">
-  <autoFilter ref="A12:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A12:C20" totalsRowShown="0">
+  <autoFilter ref="A12:C20"/>
   <tableColumns count="3">
     <tableColumn id="1" name="DrinkID"/>
     <tableColumn id="2" name="DrinkName"/>
     <tableColumn id="3" name="DrinkPrice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A24:C34" totalsRowShown="0">
+  <autoFilter ref="A24:C34"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OrderID"/>
+    <tableColumn id="2" name="PatreonID"/>
+    <tableColumn id="3" name="DrinkID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,16 +477,18 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,215 +498,323 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added basketball excel database
</commit_message>
<xml_diff>
--- a/cafeExercise.xlsx
+++ b/cafeExercise.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>CafePatreons</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>OrderID</t>
-  </si>
-  <si>
-    <t>OrderPatreons</t>
   </si>
 </sst>
 </file>
@@ -466,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +611,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -625,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -636,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -647,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -658,15 +655,12 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -676,14 +670,8 @@
       <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -693,11 +681,8 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -707,11 +692,8 @@
       <c r="C26">
         <v>2</v>
       </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -721,11 +703,8 @@
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -735,11 +714,8 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -749,11 +725,8 @@
       <c r="C29">
         <v>3</v>
       </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -764,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -775,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>

</xml_diff>